<commit_message>
[feat]: finish final close report in homework-3
</commit_message>
<xml_diff>
--- a/homework-2/Apriori/dataset.xlsx
+++ b/homework-2/Apriori/dataset.xlsx
@@ -439,27 +439,27 @@
     <row r="3">
       <c r="B3" t="inlineStr">
         <is>
-          <t>{35}</t>
+          <t>{9}</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>43</v>
+        <v>225</v>
       </c>
     </row>
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>{6}</t>
+          <t>{15}</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>31</v>
+        <v>185</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>{3}</t>
+          <t>{47}</t>
         </is>
       </c>
       <c r="C5" t="n">
@@ -469,431 +469,431 @@
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>{37}</t>
+          <t>{36}</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>37</v>
+        <v>174</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>{9}</t>
+          <t>{10}</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>225</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>{11}</t>
+          <t>{46}</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>44</v>
+        <v>48</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
-          <t>{31}</t>
+          <t>{45}</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>{1}</t>
+          <t>{32}</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>156</v>
+        <v>36</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>{20}</t>
+          <t>{5}</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>{42}</t>
+          <t>{40}</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>36</v>
+        <v>42</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>{22}</t>
+          <t>{41}</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>215</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
-          <t>{10}</t>
+          <t>{43}</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>34</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15">
       <c r="B15" t="inlineStr">
         <is>
-          <t>{47}</t>
+          <t>{42}</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>34</v>
+        <v>36</v>
       </c>
     </row>
     <row r="16">
       <c r="B16" t="inlineStr">
         <is>
-          <t>{2}</t>
+          <t>{21}</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>43</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17">
       <c r="B17" t="inlineStr">
         <is>
-          <t>{39}</t>
+          <t>{14}</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>32</v>
+        <v>293</v>
       </c>
     </row>
     <row r="18">
       <c r="B18" t="inlineStr">
         <is>
-          <t>{34}</t>
+          <t>{35}</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>33</v>
+        <v>43</v>
       </c>
     </row>
     <row r="19">
       <c r="B19" t="inlineStr">
         <is>
-          <t>{17}</t>
+          <t>{1}</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>34</v>
+        <v>156</v>
       </c>
     </row>
     <row r="20">
       <c r="B20" t="inlineStr">
         <is>
-          <t>{13}</t>
+          <t>{37}</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21">
       <c r="B21" t="inlineStr">
         <is>
-          <t>{16}</t>
+          <t>{11}</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>283</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22">
       <c r="B22" t="inlineStr">
         <is>
-          <t>{15}</t>
+          <t>{34}</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>185</v>
+        <v>33</v>
       </c>
     </row>
     <row r="23">
       <c r="B23" t="inlineStr">
         <is>
-          <t>{48}</t>
+          <t>{8}</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
       <c r="B24" t="inlineStr">
         <is>
-          <t>{45}</t>
+          <t>{18}</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>32</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
       <c r="B25" t="inlineStr">
         <is>
-          <t>{25}</t>
+          <t>{12}</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>38</v>
+        <v>300</v>
       </c>
     </row>
     <row r="26">
       <c r="B26" t="inlineStr">
         <is>
-          <t>{49}</t>
+          <t>{26}</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>162</v>
+        <v>47</v>
       </c>
     </row>
     <row r="27">
       <c r="B27" t="inlineStr">
         <is>
-          <t>{21}</t>
+          <t>{31}</t>
         </is>
       </c>
       <c r="C27" t="n">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28">
       <c r="B28" t="inlineStr">
         <is>
-          <t>{18}</t>
+          <t>{0}</t>
         </is>
       </c>
       <c r="C28" t="n">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29">
       <c r="B29" t="inlineStr">
         <is>
-          <t>{14}</t>
+          <t>{29}</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>293</v>
+        <v>36</v>
       </c>
     </row>
     <row r="30">
       <c r="B30" t="inlineStr">
         <is>
-          <t>{41}</t>
+          <t>{44}</t>
         </is>
       </c>
       <c r="C30" t="n">
-        <v>51</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31">
       <c r="B31" t="inlineStr">
         <is>
-          <t>{40}</t>
+          <t>{49}</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>42</v>
+        <v>162</v>
       </c>
     </row>
     <row r="32">
       <c r="B32" t="inlineStr">
         <is>
-          <t>{36}</t>
+          <t>{20}</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>174</v>
+        <v>39</v>
       </c>
     </row>
     <row r="33">
       <c r="B33" t="inlineStr">
         <is>
-          <t>{24}</t>
+          <t>{7}</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>37</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34">
       <c r="B34" t="inlineStr">
         <is>
-          <t>{0}</t>
+          <t>{30}</t>
         </is>
       </c>
       <c r="C34" t="n">
-        <v>32</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35">
       <c r="B35" t="inlineStr">
         <is>
-          <t>{12}</t>
+          <t>{48}</t>
         </is>
       </c>
       <c r="C35" t="n">
-        <v>300</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36">
       <c r="B36" t="inlineStr">
         <is>
-          <t>{30}</t>
+          <t>{22}</t>
         </is>
       </c>
       <c r="C36" t="n">
-        <v>37</v>
+        <v>215</v>
       </c>
     </row>
     <row r="37">
       <c r="B37" t="inlineStr">
         <is>
-          <t>{26}</t>
+          <t>{27}</t>
         </is>
       </c>
       <c r="C37" t="n">
-        <v>47</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38">
       <c r="B38" t="inlineStr">
         <is>
-          <t>{46}</t>
+          <t>{13}</t>
         </is>
       </c>
       <c r="C38" t="n">
-        <v>48</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39">
       <c r="B39" t="inlineStr">
         <is>
-          <t>{33}</t>
+          <t>{3}</t>
         </is>
       </c>
       <c r="C39" t="n">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="40">
       <c r="B40" t="inlineStr">
         <is>
-          <t>{8}</t>
+          <t>{16}</t>
         </is>
       </c>
       <c r="C40" t="n">
-        <v>41</v>
+        <v>283</v>
       </c>
     </row>
     <row r="41">
       <c r="B41" t="inlineStr">
         <is>
-          <t>{44}</t>
+          <t>{33}</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>38</v>
+        <v>47</v>
       </c>
     </row>
     <row r="42">
       <c r="B42" t="inlineStr">
         <is>
-          <t>{32}</t>
+          <t>{2}</t>
         </is>
       </c>
       <c r="C42" t="n">
-        <v>36</v>
+        <v>43</v>
       </c>
     </row>
     <row r="43">
       <c r="B43" t="inlineStr">
         <is>
-          <t>{43}</t>
+          <t>{23}</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="44">
       <c r="B44" t="inlineStr">
         <is>
-          <t>{27}</t>
+          <t>{24}</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45">
       <c r="B45" t="inlineStr">
         <is>
-          <t>{23}</t>
+          <t>{6}</t>
         </is>
       </c>
       <c r="C45" t="n">
-        <v>41</v>
+        <v>31</v>
       </c>
     </row>
     <row r="46">
       <c r="B46" t="inlineStr">
         <is>
-          <t>{28}</t>
+          <t>{39}</t>
         </is>
       </c>
       <c r="C46" t="n">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47">
       <c r="B47" t="inlineStr">
         <is>
-          <t>{5}</t>
+          <t>{17}</t>
         </is>
       </c>
       <c r="C47" t="n">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="48">
       <c r="B48" t="inlineStr">
         <is>
-          <t>{7}</t>
+          <t>{25}</t>
         </is>
       </c>
       <c r="C48" t="n">
-        <v>42</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49">
@@ -909,11 +909,11 @@
     <row r="50">
       <c r="B50" t="inlineStr">
         <is>
-          <t>{29}</t>
+          <t>{28}</t>
         </is>
       </c>
       <c r="C50" t="n">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -960,51 +960,51 @@
     <row r="4">
       <c r="B4" t="inlineStr">
         <is>
-          <t>{1, 49}</t>
+          <t>{15, 36}</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>127</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>{16, 14}</t>
+          <t>{14, 12}</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>258</v>
+        <v>268</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>{16, 12}</t>
+          <t>{14, 16}</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>{15, 36}</t>
+          <t>{1, 49}</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>139</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
-          <t>{14, 12}</t>
+          <t>{12, 16}</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
   </sheetData>
@@ -1117,151 +1117,151 @@
     <row r="5">
       <c r="B5" t="inlineStr">
         <is>
-          <t>{1}</t>
+          <t>{15}</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>{49}</t>
+          <t>{36}</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>0.8141025641025641</v>
+        <v>0.7513513513513513</v>
       </c>
     </row>
     <row r="6">
       <c r="B6" t="inlineStr">
         <is>
-          <t>{49}</t>
+          <t>{36}</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>{1}</t>
+          <t>{15}</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>0.7839506172839507</v>
+        <v>0.7988505747126436</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" t="inlineStr">
         <is>
-          <t>{16}</t>
+          <t>{14}</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>{14}</t>
+          <t>{12}</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>0.911660777385159</v>
+        <v>0.9146757679180887</v>
       </c>
     </row>
     <row r="8">
       <c r="B8" t="inlineStr">
         <is>
+          <t>{12}</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
           <t>{14}</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>{16}</t>
-        </is>
-      </c>
       <c r="D8" t="n">
-        <v>0.8805460750853242</v>
+        <v>0.8933333333333333</v>
       </c>
     </row>
     <row r="9">
       <c r="B9" t="inlineStr">
         <is>
+          <t>{14}</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
           <t>{16}</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>{12}</t>
-        </is>
-      </c>
       <c r="D9" t="n">
-        <v>0.9151943462897526</v>
+        <v>0.8805460750853242</v>
       </c>
     </row>
     <row r="10">
       <c r="B10" t="inlineStr">
         <is>
-          <t>{12}</t>
+          <t>{16}</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>{16}</t>
+          <t>{14}</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.8633333333333333</v>
+        <v>0.911660777385159</v>
       </c>
     </row>
     <row r="11">
       <c r="B11" t="inlineStr">
         <is>
-          <t>{15}</t>
+          <t>{1}</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>{36}</t>
+          <t>{49}</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>0.7513513513513513</v>
+        <v>0.8141025641025641</v>
       </c>
     </row>
     <row r="12">
       <c r="B12" t="inlineStr">
         <is>
-          <t>{36}</t>
+          <t>{49}</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>{15}</t>
+          <t>{1}</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>0.7988505747126436</v>
+        <v>0.7839506172839507</v>
       </c>
     </row>
     <row r="13">
       <c r="B13" t="inlineStr">
         <is>
-          <t>{14}</t>
+          <t>{12}</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>{12}</t>
+          <t>{16}</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>0.9146757679180887</v>
+        <v>0.8633333333333333</v>
       </c>
     </row>
     <row r="14">
       <c r="B14" t="inlineStr">
         <is>
+          <t>{16}</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
           <t>{12}</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>{14}</t>
-        </is>
-      </c>
       <c r="D14" t="n">
-        <v>0.8933333333333333</v>
+        <v>0.9151943462897526</v>
       </c>
     </row>
     <row r="15">

</xml_diff>